<commit_message>
added k64F connection .pdf
</commit_message>
<xml_diff>
--- a/micro_mirror/FRDM-K64F_PKG-mirror.xlsx
+++ b/micro_mirror/FRDM-K64F_PKG-mirror.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17736" windowHeight="8412" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17736" windowHeight="8412" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Release Note" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="509">
   <si>
     <t>A3</t>
   </si>
@@ -1510,9 +1510,6 @@
     <t>mirror board</t>
   </si>
   <si>
-    <t>Function</t>
-  </si>
-  <si>
     <t>V_SENSE_0</t>
   </si>
   <si>
@@ -1528,9 +1525,6 @@
     <t>HV_SENSE</t>
   </si>
   <si>
-    <t>function</t>
-  </si>
-  <si>
     <t>PWM_0</t>
   </si>
   <si>
@@ -1553,13 +1547,22 @@
   </si>
   <si>
     <t>SD_3</t>
+  </si>
+  <si>
+    <t>backup version</t>
+  </si>
+  <si>
+    <t>K64F IO</t>
+  </si>
+  <si>
+    <t>mirror Function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1598,8 +1601,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1654,6 +1665,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1682,7 +1699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1840,6 +1857,12 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1921,6 +1944,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3300"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FFF5C387"/>
       <color rgb="FFCC00CC"/>
@@ -17550,8 +17574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17561,18 +17585,18 @@
     <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>409</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="61" t="s">
         <v>492</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>507</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>8</v>
@@ -17616,7 +17640,7 @@
         <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>159</v>
@@ -17690,7 +17714,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>160</v>
@@ -17803,7 +17827,7 @@
         <v>57</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>167</v>
@@ -17875,7 +17899,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D9" s="50" t="s">
         <v>54</v>
@@ -17951,7 +17975,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>165</v>
@@ -17987,7 +18011,9 @@
       <c r="B12" s="2">
         <v>70</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>506</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
         <v>183</v>
@@ -18027,7 +18053,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D13" s="50" t="s">
         <v>145</v>
@@ -18103,7 +18129,7 @@
         <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D15" s="51" t="s">
         <v>63</v>
@@ -18185,7 +18211,7 @@
         <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D17" s="51" t="s">
         <v>83</v>
@@ -18234,7 +18260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -18846,8 +18872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18857,18 +18883,18 @@
     <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="17" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="17" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>409</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>493</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>492</v>
+      <c r="C1" s="61" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" s="62" t="s">
+        <v>507</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>8</v>
@@ -18941,7 +18967,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D3" s="55" t="s">
         <v>240</v>
@@ -19011,7 +19037,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D5" s="55" t="s">
         <v>241</v>
@@ -19081,7 +19107,7 @@
         <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D7" s="55" t="s">
         <v>253</v>
@@ -19151,7 +19177,7 @@
         <v>59</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D9" s="55" t="s">
         <v>254</v>
@@ -19225,7 +19251,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D11" s="55" t="s">
         <v>258</v>

</xml_diff>